<commit_message>
Add a wait before updating the notebook if a new excel is imported
</commit_message>
<xml_diff>
--- a/app/code/data/excels/raw_copy_expenses.xlsx
+++ b/app/code/data/excels/raw_copy_expenses.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1614374801" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1614374801" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1614374801" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1614374801"/>
+      <pm:revision xmlns:pm="smNativeData" day="1614466693" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1614466693" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1614466693" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1614466693"/>
     </ext>
   </extLst>
 </workbook>
@@ -1273,7 +1273,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614374801" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1288,7 +1288,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614374801" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1304,7 +1304,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614374801" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1319,7 +1319,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614374801" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1376,7 +1376,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801"/>
+          <pm:border xmlns:pm="smNativeData" id="1614466693"/>
         </ext>
       </extLst>
     </border>
@@ -1395,7 +1395,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1416,7 +1416,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1438,7 +1438,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1459,7 +1459,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1480,7 +1480,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1502,7 +1502,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1525,7 +1525,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1547,7 +1547,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614374801">
+          <pm:border xmlns:pm="smNativeData" id="1614466693">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1628,10 +1628,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1614374801" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1614466693" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1614374801" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1614466693" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -1898,7 +1898,7 @@
   <dimension ref="A1:K624"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G9"/>
+      <selection activeCell="B2" sqref="B2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -9886,7 +9886,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614374801" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9895,14 +9895,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614374801" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9924,7 +9924,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614374801" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9933,14 +9933,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614374801" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9962,7 +9962,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614374801" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9971,14 +9971,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614374801" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614374801" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>